<commit_message>
created a nix file for running this analysis reproducably
</commit_message>
<xml_diff>
--- a/data/output/tableau_upload.xlsx
+++ b/data/output/tableau_upload.xlsx
@@ -10,7 +10,8 @@
     <sheet name="md_data" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="va_data" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="national_data" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="national.monthly.strikes" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="year.strikes.2024.monthly" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="year.strikes.2023.monthly" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -425,6 +426,23 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2024</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -639,7 +657,7 @@
         <v>2021</v>
       </c>
       <c r="B2" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" t="n">
         <v>211</v>
@@ -667,13 +685,13 @@
         <v>2023</v>
       </c>
       <c r="B4" t="n">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C4" t="n">
         <v>320</v>
       </c>
       <c r="D4" t="n">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="5">
@@ -681,13 +699,13 @@
         <v>2024</v>
       </c>
       <c r="B5" t="n">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C5" t="n">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="D5" t="n">
-        <v>193</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -737,13 +755,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C3" t="n">
         <v>14</v>
       </c>
-      <c r="C3" t="n">
-        <v>16</v>
-      </c>
       <c r="D3" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -751,13 +769,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D4" t="n">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5">
@@ -765,13 +783,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D5" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
@@ -779,13 +797,223 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
+        <v>32</v>
+      </c>
+      <c r="C6" t="n">
+        <v>46</v>
+      </c>
+      <c r="D6" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>40</v>
+      </c>
+      <c r="C2" t="n">
+        <v>69</v>
+      </c>
+      <c r="D2" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>9</v>
+      </c>
+      <c r="C3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>19</v>
+      </c>
+      <c r="C4" t="n">
+        <v>26</v>
+      </c>
+      <c r="D4" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>22</v>
+      </c>
+      <c r="C5" t="n">
+        <v>31</v>
+      </c>
+      <c r="D5" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>16</v>
+      </c>
+      <c r="C6" t="n">
+        <v>29</v>
+      </c>
+      <c r="D6" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>20</v>
+      </c>
+      <c r="C7" t="n">
+        <v>27</v>
+      </c>
+      <c r="D7" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>15</v>
+      </c>
+      <c r="C8" t="n">
+        <v>22</v>
+      </c>
+      <c r="D8" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>14</v>
+      </c>
+      <c r="C9" t="n">
+        <v>25</v>
+      </c>
+      <c r="D9" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>23</v>
+      </c>
+      <c r="C10" t="n">
+        <v>33</v>
+      </c>
+      <c r="D10" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>21</v>
+      </c>
+      <c r="C11" t="n">
+        <v>32</v>
+      </c>
+      <c r="D11" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>24</v>
+      </c>
+      <c r="C12" t="n">
+        <v>36</v>
+      </c>
+      <c r="D12" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
         <v>12</v>
       </c>
-      <c r="C6" t="n">
-        <v>14</v>
-      </c>
-      <c r="D6" t="n">
-        <v>14</v>
+      <c r="B13" t="n">
+        <v>28</v>
+      </c>
+      <c r="C13" t="n">
+        <v>39</v>
+      </c>
+      <c r="D13" t="n">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added in shiny app for more testing
</commit_message>
<xml_diff>
--- a/data/output/tableau_upload.xlsx
+++ b/data/output/tableau_upload.xlsx
@@ -576,13 +576,13 @@
         <v>2024</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -667,6 +667,23 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2024</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -802,10 +819,10 @@
         <v>90</v>
       </c>
       <c r="C2" t="n">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D2" t="n">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3">
@@ -827,13 +844,13 @@
         <v>2023</v>
       </c>
       <c r="B4" t="n">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C4" t="n">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="D4" t="n">
-        <v>473</v>
+        <v>466</v>
       </c>
     </row>
     <row r="5">
@@ -841,13 +858,13 @@
         <v>2024</v>
       </c>
       <c r="B5" t="n">
-        <v>86</v>
+        <v>133</v>
       </c>
       <c r="C5" t="n">
-        <v>165</v>
+        <v>272</v>
       </c>
       <c r="D5" t="n">
-        <v>230</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -914,10 +931,10 @@
         <v>20</v>
       </c>
       <c r="C4" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5">
@@ -925,13 +942,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="n">
+        <v>25</v>
+      </c>
+      <c r="D5" t="n">
         <v>26</v>
-      </c>
-      <c r="D5" t="n">
-        <v>27</v>
       </c>
     </row>
     <row r="6">
@@ -939,13 +956,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D6" t="n">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7">
@@ -953,13 +970,69 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>24</v>
+      </c>
+      <c r="C8" t="n">
+        <v>37</v>
+      </c>
+      <c r="D8" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>18</v>
+      </c>
+      <c r="C9" t="n">
+        <v>24</v>
+      </c>
+      <c r="D9" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>18</v>
+      </c>
+      <c r="C10" t="n">
+        <v>33</v>
+      </c>
+      <c r="D10" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>13</v>
+      </c>
+      <c r="C11" t="n">
+        <v>17</v>
+      </c>
+      <c r="D11" t="n">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1009,13 +1082,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
         <v>9</v>
       </c>
-      <c r="C3" t="n">
-        <v>10</v>
-      </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -1037,13 +1110,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
@@ -1054,10 +1127,10 @@
         <v>16</v>
       </c>
       <c r="C6" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7">
@@ -1065,13 +1138,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="n">
+        <v>26</v>
+      </c>
+      <c r="D7" t="n">
         <v>27</v>
-      </c>
-      <c r="D7" t="n">
-        <v>28</v>
       </c>
     </row>
     <row r="8">
@@ -1096,10 +1169,10 @@
         <v>14</v>
       </c>
       <c r="C9" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10">
@@ -1110,10 +1183,10 @@
         <v>23</v>
       </c>
       <c r="C10" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D10" t="n">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11">
@@ -1248,13 +1321,13 @@
         <v>2024</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -1395,19 +1468,19 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C14" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -1415,16 +1488,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C15" t="n">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D15" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="E15" t="n">
-        <v>64</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16">
@@ -1432,16 +1505,16 @@
         <v>13</v>
       </c>
       <c r="B16" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C16" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D16" t="n">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E16" t="n">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17">
@@ -1449,33 +1522,33 @@
         <v>13</v>
       </c>
       <c r="B17" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C17" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D17" t="n">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="E17" t="n">
-        <v>48</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19">
@@ -1483,16 +1556,16 @@
         <v>14</v>
       </c>
       <c r="B19" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -1500,7 +1573,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C20" t="n">
         <v>3</v>
@@ -1517,33 +1590,33 @@
         <v>14</v>
       </c>
       <c r="B21" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C21" t="n">
         <v>3</v>
       </c>
       <c r="D21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C22" t="n">
         <v>3</v>
       </c>
       <c r="D22" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23">
@@ -1551,10 +1624,10 @@
         <v>15</v>
       </c>
       <c r="B23" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D23" t="n">
         <v>3</v>
@@ -1568,16 +1641,16 @@
         <v>15</v>
       </c>
       <c r="B24" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C24" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D24" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25">
@@ -1585,50 +1658,50 @@
         <v>15</v>
       </c>
       <c r="B25" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C25" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D25" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B27" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1636,16 +1709,16 @@
         <v>5</v>
       </c>
       <c r="B28" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
@@ -1653,33 +1726,33 @@
         <v>5</v>
       </c>
       <c r="B29" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B30" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C30" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D30" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
@@ -1687,16 +1760,16 @@
         <v>17</v>
       </c>
       <c r="B31" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C31" t="n">
         <v>2</v>
       </c>
       <c r="D31" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -1704,16 +1777,16 @@
         <v>17</v>
       </c>
       <c r="B32" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33">
@@ -1721,33 +1794,33 @@
         <v>17</v>
       </c>
       <c r="B33" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B34" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -1755,16 +1828,16 @@
         <v>18</v>
       </c>
       <c r="B35" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C35" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
@@ -1772,7 +1845,7 @@
         <v>18</v>
       </c>
       <c r="B36" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C36" t="n">
         <v>3</v>
@@ -1781,7 +1854,7 @@
         <v>4</v>
       </c>
       <c r="E36" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37">
@@ -1789,33 +1862,33 @@
         <v>18</v>
       </c>
       <c r="B37" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C37" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D37" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B38" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D38" t="n">
         <v>3</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
@@ -1823,50 +1896,50 @@
         <v>19</v>
       </c>
       <c r="B39" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C39" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D39" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B40" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B41" t="n">
         <v>2021</v>
       </c>
       <c r="C41" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E41" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1874,16 +1947,16 @@
         <v>21</v>
       </c>
       <c r="B42" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C42" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D42" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E42" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43">
@@ -1891,16 +1964,16 @@
         <v>21</v>
       </c>
       <c r="B43" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C43" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D43" t="n">
+        <v>15</v>
+      </c>
+      <c r="E43" t="n">
         <v>19</v>
-      </c>
-      <c r="E43" t="n">
-        <v>23</v>
       </c>
     </row>
     <row r="44">
@@ -1908,33 +1981,33 @@
         <v>21</v>
       </c>
       <c r="B44" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C44" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D44" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E44" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B45" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C45" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D45" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46">
@@ -1942,16 +2015,16 @@
         <v>22</v>
       </c>
       <c r="B46" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C46" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D46" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47">
@@ -1959,16 +2032,16 @@
         <v>22</v>
       </c>
       <c r="B47" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C47" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D47" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48">
@@ -1976,33 +2049,33 @@
         <v>22</v>
       </c>
       <c r="B48" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B49" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C49" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D49" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50">
@@ -2010,16 +2083,16 @@
         <v>23</v>
       </c>
       <c r="B50" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C50" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D50" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51">
@@ -2027,33 +2100,33 @@
         <v>23</v>
       </c>
       <c r="B51" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B52" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C52" t="n">
         <v>2</v>
       </c>
       <c r="D52" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53">
@@ -2061,7 +2134,7 @@
         <v>24</v>
       </c>
       <c r="B53" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C53" t="n">
         <v>2</v>
@@ -2070,7 +2143,7 @@
         <v>2</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
@@ -2078,33 +2151,33 @@
         <v>24</v>
       </c>
       <c r="B54" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B55" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -2112,16 +2185,16 @@
         <v>25</v>
       </c>
       <c r="B56" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57">
@@ -2129,7 +2202,7 @@
         <v>25</v>
       </c>
       <c r="B57" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C57" t="n">
         <v>1</v>
@@ -2138,7 +2211,7 @@
         <v>3</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58">
@@ -2146,33 +2219,33 @@
         <v>25</v>
       </c>
       <c r="B58" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C58" t="n">
         <v>1</v>
       </c>
       <c r="D58" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B59" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C59" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D59" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60">
@@ -2180,16 +2253,16 @@
         <v>26</v>
       </c>
       <c r="B60" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D60" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61">
@@ -2197,16 +2270,16 @@
         <v>26</v>
       </c>
       <c r="B61" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C61" t="n">
         <v>2</v>
       </c>
       <c r="D61" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62">
@@ -2214,33 +2287,33 @@
         <v>26</v>
       </c>
       <c r="B62" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D62" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B63" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
@@ -2248,16 +2321,16 @@
         <v>27</v>
       </c>
       <c r="B64" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65">
@@ -2265,33 +2338,33 @@
         <v>27</v>
       </c>
       <c r="B65" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C65" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B66" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D66" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -2299,16 +2372,16 @@
         <v>6</v>
       </c>
       <c r="B67" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C67" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D67" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68">
@@ -2316,50 +2389,50 @@
         <v>6</v>
       </c>
       <c r="B68" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C68" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D68" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B69" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C69" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D69" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B70" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C70" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D70" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E70" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -2367,16 +2440,16 @@
         <v>28</v>
       </c>
       <c r="B71" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C71" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D71" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E71" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72">
@@ -2384,47 +2457,47 @@
         <v>28</v>
       </c>
       <c r="B72" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C72" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D72" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B73" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C73" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D73" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B74" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C74" t="n">
+        <v>8</v>
+      </c>
+      <c r="D74" t="n">
         <v>6</v>
-      </c>
-      <c r="D74" t="n">
-        <v>8</v>
       </c>
       <c r="E74" t="n">
         <v>10</v>
@@ -2435,16 +2508,16 @@
         <v>29</v>
       </c>
       <c r="B75" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C75" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D75" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76">
@@ -2452,50 +2525,50 @@
         <v>29</v>
       </c>
       <c r="B76" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C76" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D76" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B77" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C77" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D77" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B78" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C78" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D78" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79">
@@ -2503,16 +2576,16 @@
         <v>30</v>
       </c>
       <c r="B79" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C79" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D79" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E79" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80">
@@ -2520,50 +2593,50 @@
         <v>30</v>
       </c>
       <c r="B80" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C80" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D80" t="n">
+        <v>5</v>
+      </c>
+      <c r="E80" t="n">
         <v>6</v>
-      </c>
-      <c r="E80" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B81" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B82" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D82" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83">
@@ -2571,16 +2644,16 @@
         <v>31</v>
       </c>
       <c r="B83" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D83" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84">
@@ -2588,50 +2661,50 @@
         <v>31</v>
       </c>
       <c r="B84" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D84" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B85" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C85" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D85" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B86" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C86" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D86" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87">
@@ -2639,16 +2712,16 @@
         <v>32</v>
       </c>
       <c r="B87" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C87" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D87" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E87" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="88">
@@ -2656,101 +2729,101 @@
         <v>32</v>
       </c>
       <c r="B88" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C88" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E88" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B89" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D89" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B90" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D90" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B91" t="n">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="C91" t="n">
         <v>1</v>
       </c>
       <c r="D91" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B92" t="n">
         <v>2021</v>
       </c>
       <c r="C92" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D92" t="n">
         <v>1</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B93" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94">
@@ -2758,16 +2831,16 @@
         <v>35</v>
       </c>
       <c r="B94" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D94" t="n">
         <v>1</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95">
@@ -2775,67 +2848,67 @@
         <v>35</v>
       </c>
       <c r="B95" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C95" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D95" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B96" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C96" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D96" t="n">
         <v>1</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B97" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C97" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D97" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B98" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C98" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D98" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -2843,16 +2916,16 @@
         <v>37</v>
       </c>
       <c r="B99" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D99" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100">
@@ -2860,84 +2933,84 @@
         <v>37</v>
       </c>
       <c r="B100" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C100" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D100" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E100" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B101" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C101" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D101" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E101" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B102" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D102" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E102" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B103" t="n">
         <v>2021</v>
       </c>
       <c r="C103" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D103" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E103" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B104" t="n">
         <v>2022</v>
       </c>
       <c r="C104" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D104" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E104" t="n">
-        <v>33</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -2945,16 +3018,16 @@
         <v>39</v>
       </c>
       <c r="B105" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C105" t="n">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D105" t="n">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E105" t="n">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="106">
@@ -2962,50 +3035,50 @@
         <v>39</v>
       </c>
       <c r="B106" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C106" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D106" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E106" t="n">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B107" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C107" t="n">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D107" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E107" t="n">
-        <v>10</v>
+        <v>46</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B108" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C108" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D108" t="n">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E108" t="n">
-        <v>6</v>
+        <v>34</v>
       </c>
     </row>
     <row r="109">
@@ -3013,16 +3086,16 @@
         <v>40</v>
       </c>
       <c r="B109" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C109" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D109" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E109" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110">
@@ -3030,13 +3103,13 @@
         <v>40</v>
       </c>
       <c r="B110" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C110" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D110" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E110" t="n">
         <v>6</v>
@@ -3044,53 +3117,53 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B111" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C111" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D111" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E111" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B112" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C112" t="n">
         <v>5</v>
       </c>
       <c r="D112" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E112" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B113" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C113" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D113" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E113" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">
@@ -3098,16 +3171,16 @@
         <v>42</v>
       </c>
       <c r="B114" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C114" t="n">
+        <v>5</v>
+      </c>
+      <c r="D114" t="n">
         <v>7</v>
       </c>
-      <c r="D114" t="n">
-        <v>8</v>
-      </c>
       <c r="E114" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="115">
@@ -3115,67 +3188,67 @@
         <v>42</v>
       </c>
       <c r="B115" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C115" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D115" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E115" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B116" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C116" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D116" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E116" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B117" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C117" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D117" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E117" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B118" t="n">
         <v>2022</v>
       </c>
       <c r="C118" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D118" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E118" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119">
@@ -3183,16 +3256,16 @@
         <v>44</v>
       </c>
       <c r="B119" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C119" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D119" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E119" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120">
@@ -3200,13 +3273,13 @@
         <v>44</v>
       </c>
       <c r="B120" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C120" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D120" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E120" t="n">
         <v>5</v>
@@ -3214,36 +3287,36 @@
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B121" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C121" t="n">
         <v>8</v>
       </c>
       <c r="D121" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E121" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B122" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C122" t="n">
+        <v>4</v>
+      </c>
+      <c r="D122" t="n">
+        <v>4</v>
+      </c>
+      <c r="E122" t="n">
         <v>6</v>
-      </c>
-      <c r="D122" t="n">
-        <v>7</v>
-      </c>
-      <c r="E122" t="n">
-        <v>10</v>
       </c>
     </row>
     <row r="123">
@@ -3251,16 +3324,16 @@
         <v>45</v>
       </c>
       <c r="B123" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C123" t="n">
         <v>8</v>
       </c>
       <c r="D123" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E123" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="124">
@@ -3268,50 +3341,50 @@
         <v>45</v>
       </c>
       <c r="B124" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C124" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D124" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E124" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B125" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C125" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D125" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E125" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B126" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C126" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D126" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E126" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="127">
@@ -3319,16 +3392,16 @@
         <v>46</v>
       </c>
       <c r="B127" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C127" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D127" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E127" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128">
@@ -3336,7 +3409,7 @@
         <v>46</v>
       </c>
       <c r="B128" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C128" t="n">
         <v>1</v>
@@ -3350,10 +3423,10 @@
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B129" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C129" t="n">
         <v>3</v>
@@ -3367,64 +3440,64 @@
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B130" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C130" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D130" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E130" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B131" t="n">
         <v>2021</v>
       </c>
       <c r="C131" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D131" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E131" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B132" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C132" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D132" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E132" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B133" t="n">
         <v>2024</v>
       </c>
       <c r="C133" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D133" t="n">
         <v>3</v>
@@ -3435,47 +3508,47 @@
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B134" t="n">
         <v>2021</v>
       </c>
       <c r="C134" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D134" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E134" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B135" t="n">
         <v>2022</v>
       </c>
       <c r="C135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D135" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E135" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B136" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C136" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D136" t="n">
         <v>4</v>
@@ -3489,24 +3562,24 @@
         <v>49</v>
       </c>
       <c r="B137" t="n">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="C137" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D137" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E137" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B138" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C138" t="n">
         <v>1</v>
@@ -3515,41 +3588,41 @@
         <v>2</v>
       </c>
       <c r="E138" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B139" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C139" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D139" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E139" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B140" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C140" t="n">
+        <v>5</v>
+      </c>
+      <c r="D140" t="n">
+        <v>6</v>
+      </c>
+      <c r="E140" t="n">
         <v>7</v>
-      </c>
-      <c r="D140" t="n">
-        <v>8</v>
-      </c>
-      <c r="E140" t="n">
-        <v>13</v>
       </c>
     </row>
     <row r="141">
@@ -3557,78 +3630,78 @@
         <v>50</v>
       </c>
       <c r="B141" t="n">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="C141" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D141" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E141" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B142" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C142" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D142" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E142" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B143" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C143" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D143" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E143" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B144" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C144" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D144" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E144" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B145" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C145" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D145" t="n">
         <v>1</v>
@@ -3639,53 +3712,53 @@
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="B146" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C146" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D146" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E146" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B147" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C147" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D147" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E147" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B148" t="n">
         <v>2023</v>
       </c>
       <c r="C148" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D148" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E148" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149">
@@ -3693,67 +3766,67 @@
         <v>7</v>
       </c>
       <c r="B149" t="n">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="C149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D149" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E149" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="B150" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C150" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D150" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E150" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="B151" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C151" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D151" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E151" t="n">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="B152" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C152" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D152" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E152" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="153">
@@ -3761,118 +3834,186 @@
         <v>53</v>
       </c>
       <c r="B153" t="n">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="C153" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D153" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E153" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B154" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C154" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D154" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E154" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B155" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C155" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D155" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E155" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B156" t="n">
         <v>2024</v>
       </c>
       <c r="C156" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D156" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E156" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B157" t="n">
         <v>2021</v>
       </c>
       <c r="C157" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D157" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E157" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B158" t="n">
         <v>2022</v>
       </c>
       <c r="C158" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D158" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E158" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
+        <v>54</v>
+      </c>
+      <c r="B159" t="n">
+        <v>2024</v>
+      </c>
+      <c r="C159" t="n">
+        <v>1</v>
+      </c>
+      <c r="D159" t="n">
+        <v>1</v>
+      </c>
+      <c r="E159" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
         <v>55</v>
       </c>
-      <c r="B159" t="n">
-        <v>2023</v>
-      </c>
-      <c r="C159" t="n">
-        <v>4</v>
-      </c>
-      <c r="D159" t="n">
-        <v>5</v>
-      </c>
-      <c r="E159" t="n">
+      <c r="B160" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C160" t="n">
+        <v>3</v>
+      </c>
+      <c r="D160" t="n">
+        <v>4</v>
+      </c>
+      <c r="E160" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>55</v>
+      </c>
+      <c r="B161" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C161" t="n">
+        <v>2</v>
+      </c>
+      <c r="D161" t="n">
+        <v>2</v>
+      </c>
+      <c r="E161" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>55</v>
+      </c>
+      <c r="B162" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C162" t="n">
+        <v>4</v>
+      </c>
+      <c r="D162" t="n">
+        <v>5</v>
+      </c>
+      <c r="E162" t="n">
         <v>6</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>55</v>
+      </c>
+      <c r="B163" t="n">
+        <v>2024</v>
+      </c>
+      <c r="C163" t="n">
+        <v>2</v>
+      </c>
+      <c r="D163" t="n">
+        <v>2</v>
+      </c>
+      <c r="E163" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added more data and updated function
</commit_message>
<xml_diff>
--- a/data/output/tableau_upload.xlsx
+++ b/data/output/tableau_upload.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t xml:space="preserve">State</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t xml:space="preserve">Wisconsin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wyoming</t>
   </si>
 </sst>
 </file>
@@ -675,13 +678,30 @@
         <v>2024</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -783,6 +803,23 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -850,7 +887,7 @@
         <v>313</v>
       </c>
       <c r="D4" t="n">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="5">
@@ -858,13 +895,27 @@
         <v>2024</v>
       </c>
       <c r="B5" t="n">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="C5" t="n">
-        <v>272</v>
+        <v>306</v>
       </c>
       <c r="D5" t="n">
-        <v>359</v>
+        <v>403</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2025</v>
+      </c>
+      <c r="B6" t="n">
+        <v>28</v>
+      </c>
+      <c r="C6" t="n">
+        <v>55</v>
+      </c>
+      <c r="D6" t="n">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -903,10 +954,10 @@
         <v>33</v>
       </c>
       <c r="C2" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" t="n">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3">
@@ -914,13 +965,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -928,13 +979,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -956,13 +1007,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" t="n">
         <v>37</v>
       </c>
       <c r="D6" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7">
@@ -973,10 +1024,10 @@
         <v>18</v>
       </c>
       <c r="C7" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -984,13 +1035,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C8" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D8" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9">
@@ -998,13 +1049,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
+        <v>13</v>
+      </c>
+      <c r="C9" t="n">
+        <v>16</v>
+      </c>
+      <c r="D9" t="n">
         <v>18</v>
-      </c>
-      <c r="C9" t="n">
-        <v>24</v>
-      </c>
-      <c r="D9" t="n">
-        <v>26</v>
       </c>
     </row>
     <row r="10">
@@ -1012,13 +1063,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" t="n">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D10" t="n">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
@@ -1026,13 +1077,41 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C11" t="n">
+        <v>21</v>
+      </c>
+      <c r="D11" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
         <v>17</v>
       </c>
-      <c r="D11" t="n">
-        <v>17</v>
+      <c r="C12" t="n">
+        <v>26</v>
+      </c>
+      <c r="D12" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>21</v>
+      </c>
+      <c r="C13" t="n">
+        <v>39</v>
+      </c>
+      <c r="D13" t="n">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1158,7 +1237,7 @@
         <v>22</v>
       </c>
       <c r="D8" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9">
@@ -1426,27 +1505,27 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>2021</v>
+        <v>2025</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
         <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -1454,16 +1533,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -1471,33 +1550,33 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C15" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -1505,16 +1584,16 @@
         <v>13</v>
       </c>
       <c r="B16" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C16" t="n">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D16" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="E16" t="n">
-        <v>64</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17">
@@ -1522,16 +1601,16 @@
         <v>13</v>
       </c>
       <c r="B17" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C17" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D17" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E17" t="n">
-        <v>82</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18">
@@ -1539,50 +1618,50 @@
         <v>13</v>
       </c>
       <c r="B18" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C18" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D18" t="n">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E18" t="n">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" t="n">
-        <v>2022</v>
+        <v>2025</v>
       </c>
       <c r="C20" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D20" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21">
@@ -1590,16 +1669,16 @@
         <v>14</v>
       </c>
       <c r="B21" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
@@ -1607,24 +1686,24 @@
         <v>14</v>
       </c>
       <c r="B22" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C22" t="n">
         <v>3</v>
       </c>
       <c r="D22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C23" t="n">
         <v>3</v>
@@ -1638,36 +1717,36 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D24" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B25" t="n">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="C25" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1675,112 +1754,112 @@
         <v>15</v>
       </c>
       <c r="B26" t="n">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="C26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C28" t="n">
+        <v>4</v>
+      </c>
+      <c r="D28" t="n">
         <v>5</v>
       </c>
-      <c r="B28" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C28" t="n">
-        <v>3</v>
-      </c>
-      <c r="D28" t="n">
-        <v>4</v>
-      </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B29" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C29" t="n">
         <v>2</v>
       </c>
       <c r="D29" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B30" t="n">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="C30" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31" t="n">
         <v>2021</v>
       </c>
       <c r="C31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B32" t="n">
         <v>2022</v>
       </c>
       <c r="C32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32" t="n">
         <v>4</v>
@@ -1791,13 +1870,13 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B33" t="n">
         <v>2023</v>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33" t="n">
         <v>3</v>
@@ -1808,30 +1887,30 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B34" t="n">
         <v>2024</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35" t="n">
         <v>2021</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D35" t="n">
         <v>2</v>
@@ -1842,370 +1921,370 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B36" t="n">
         <v>2022</v>
       </c>
       <c r="C36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D36" t="n">
         <v>4</v>
       </c>
       <c r="E36" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B37" t="n">
         <v>2023</v>
       </c>
       <c r="C37" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B38" t="n">
         <v>2024</v>
       </c>
       <c r="C38" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B39" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C39" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B40" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D40" t="n">
         <v>4</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B41" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C41" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D41" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B42" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C42" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D42" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B43" t="n">
-        <v>2022</v>
+        <v>2025</v>
       </c>
       <c r="C43" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D43" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E43" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B44" t="n">
         <v>2023</v>
       </c>
       <c r="C44" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D44" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E44" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B45" t="n">
         <v>2024</v>
       </c>
       <c r="C45" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D45" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E45" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B46" t="n">
-        <v>2021</v>
+        <v>2025</v>
       </c>
       <c r="C46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D46" t="n">
         <v>4</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B47" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C47" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D47" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B48" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C48" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D48" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B49" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C49" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D49" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B50" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C50" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D50" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B51" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C51" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D51" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B52" t="n">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="C52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B53" t="n">
         <v>2021</v>
       </c>
       <c r="C53" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D53" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B54" t="n">
         <v>2022</v>
       </c>
       <c r="C54" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D54" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B55" t="n">
         <v>2023</v>
       </c>
       <c r="C55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B56" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C56" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D56" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B57" t="n">
         <v>2022</v>
       </c>
       <c r="C57" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D57" t="n">
         <v>3</v>
@@ -2216,47 +2295,47 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B58" t="n">
         <v>2023</v>
       </c>
       <c r="C58" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D58" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B59" t="n">
         <v>2024</v>
       </c>
       <c r="C59" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D59" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B60" t="n">
         <v>2021</v>
       </c>
       <c r="C60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D60" t="n">
         <v>2</v>
@@ -2267,7 +2346,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B61" t="n">
         <v>2022</v>
@@ -2276,49 +2355,49 @@
         <v>2</v>
       </c>
       <c r="D61" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B62" t="n">
         <v>2023</v>
       </c>
       <c r="C62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D62" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B63" t="n">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B64" t="n">
         <v>2022</v>
@@ -2327,21 +2406,21 @@
         <v>1</v>
       </c>
       <c r="D64" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B65" t="n">
         <v>2023</v>
       </c>
       <c r="C65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D65" t="n">
         <v>3</v>
@@ -2352,47 +2431,47 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B66" t="n">
         <v>2024</v>
       </c>
       <c r="C66" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D66" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B67" t="n">
         <v>2021</v>
       </c>
       <c r="C67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D67" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B68" t="n">
         <v>2022</v>
       </c>
       <c r="C68" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D68" t="n">
         <v>4</v>
@@ -2403,7 +2482,7 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B69" t="n">
         <v>2023</v>
@@ -2412,15 +2491,15 @@
         <v>2</v>
       </c>
       <c r="D69" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B70" t="n">
         <v>2024</v>
@@ -2437,387 +2516,387 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B71" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C71" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D71" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B72" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C72" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D72" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E72" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B73" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C73" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D73" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E73" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B74" t="n">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="C74" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B75" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C75" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D75" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B76" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C76" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D76" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B77" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C77" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D77" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B78" t="n">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="C78" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D78" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B79" t="n">
         <v>2021</v>
       </c>
       <c r="C79" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D79" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B80" t="n">
         <v>2022</v>
       </c>
       <c r="C80" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D80" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B81" t="n">
         <v>2023</v>
       </c>
       <c r="C81" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D81" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E81" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B82" t="n">
         <v>2024</v>
       </c>
       <c r="C82" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D82" t="n">
         <v>8</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B83" t="n">
-        <v>2021</v>
+        <v>2025</v>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D83" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B84" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D84" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B85" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C85" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D85" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B86" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C86" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D86" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B87" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C87" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D87" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B88" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C88" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D88" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E88" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B89" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C89" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D89" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E89" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B90" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C90" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D90" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E90" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B91" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C91" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D91" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B92" t="n">
-        <v>2021</v>
+        <v>2025</v>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D92" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B93" t="n">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="C93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D93" t="n">
         <v>1</v>
@@ -2828,16 +2907,16 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B94" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D94" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E94" t="n">
         <v>3</v>
@@ -2845,146 +2924,146 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B95" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D95" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B96" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C96" t="n">
         <v>2</v>
       </c>
       <c r="D96" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B97" t="n">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="C97" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D97" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B98" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C98" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D98" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B99" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C99" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D99" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B100" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C100" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D100" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E100" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B101" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C101" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D101" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E101" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B102" t="n">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="C102" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D102" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E102" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B103" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C103" t="n">
         <v>1</v>
@@ -2998,10 +3077,10 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B104" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C104" t="n">
         <v>1</v>
@@ -3010,310 +3089,310 @@
         <v>1</v>
       </c>
       <c r="E104" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B105" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C105" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D105" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E105" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B106" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C106" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D106" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E106" t="n">
-        <v>33</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B107" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C107" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="D107" t="n">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="E107" t="n">
-        <v>46</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B108" t="n">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="C108" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D108" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E108" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B109" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C109" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D109" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E109" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B110" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C110" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D110" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E110" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B111" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C111" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D111" t="n">
         <v>6</v>
       </c>
       <c r="E111" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B112" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C112" t="n">
         <v>5</v>
       </c>
       <c r="D112" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E112" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B113" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C113" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D113" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E113" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B114" t="n">
         <v>2021</v>
       </c>
       <c r="C114" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D114" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E114" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B115" t="n">
         <v>2022</v>
       </c>
       <c r="C115" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D115" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E115" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B116" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C116" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D116" t="n">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E116" t="n">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B117" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C117" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D117" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E117" t="n">
-        <v>6</v>
+        <v>33</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B118" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C118" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="D118" t="n">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E118" t="n">
-        <v>2</v>
+        <v>46</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B119" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C119" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D119" t="n">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="E119" t="n">
-        <v>4</v>
+        <v>37</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B120" t="n">
-        <v>2022</v>
+        <v>2025</v>
       </c>
       <c r="C120" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D120" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E120" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B121" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C121" t="n">
+        <v>4</v>
+      </c>
+      <c r="D121" t="n">
         <v>8</v>
       </c>
-      <c r="D121" t="n">
+      <c r="E121" t="n">
         <v>10</v>
-      </c>
-      <c r="E121" t="n">
-        <v>15</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B122" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C122" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D122" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E122" t="n">
         <v>6</v>
@@ -3321,163 +3400,163 @@
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B123" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C123" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D123" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E123" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B124" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C124" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D124" t="n">
         <v>7</v>
       </c>
       <c r="E124" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B125" t="n">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="C125" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D125" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E125" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B126" t="n">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="C126" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D126" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E126" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B127" t="n">
         <v>2021</v>
       </c>
       <c r="C127" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D127" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E127" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B128" t="n">
         <v>2022</v>
       </c>
       <c r="C128" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D128" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E128" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B129" t="n">
         <v>2023</v>
       </c>
       <c r="C129" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D129" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E129" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B130" t="n">
         <v>2024</v>
       </c>
       <c r="C130" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D130" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E130" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B131" t="n">
-        <v>2021</v>
+        <v>2025</v>
       </c>
       <c r="C131" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D131" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E131" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B132" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C132" t="n">
         <v>1</v>
@@ -3486,15 +3565,15 @@
         <v>2</v>
       </c>
       <c r="E132" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B133" t="n">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="C133" t="n">
         <v>3</v>
@@ -3503,250 +3582,250 @@
         <v>3</v>
       </c>
       <c r="E133" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B134" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C134" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D134" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E134" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B135" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C135" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D135" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E135" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B136" t="n">
         <v>2024</v>
       </c>
       <c r="C136" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D136" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E136" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B137" t="n">
-        <v>2021</v>
+        <v>2025</v>
       </c>
       <c r="C137" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D137" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E137" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B138" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C138" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D138" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E138" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B139" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C139" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D139" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E139" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B140" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C140" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D140" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E140" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B141" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C141" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D141" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E141" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B142" t="n">
-        <v>2022</v>
+        <v>2025</v>
       </c>
       <c r="C142" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D142" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E142" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B143" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C143" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D143" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E143" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B144" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C144" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D144" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E144" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B145" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C145" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D145" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E145" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B146" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C146" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D146" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E146" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B147" t="n">
         <v>2021</v>
       </c>
       <c r="C147" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D147" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E147" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B148" t="n">
         <v>2023</v>
@@ -3755,38 +3834,38 @@
         <v>1</v>
       </c>
       <c r="D148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E148" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="B149" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C149" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D149" t="n">
         <v>3</v>
       </c>
       <c r="E149" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="B150" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C150" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D150" t="n">
         <v>2</v>
@@ -3797,223 +3876,597 @@
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="B151" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C151" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D151" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E151" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="B152" t="n">
         <v>2024</v>
       </c>
       <c r="C152" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D152" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E152" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B153" t="n">
-        <v>2021</v>
+        <v>2025</v>
       </c>
       <c r="C153" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D153" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E153" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B154" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C154" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D154" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E154" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B155" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C155" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D155" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E155" t="n">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B156" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C156" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D156" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E156" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B157" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C157" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D157" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E157" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B158" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C158" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D158" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E158" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B159" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C159" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D159" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E159" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B160" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C160" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D160" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E160" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B161" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C161" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D161" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E161" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B162" t="n">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="C162" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D162" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E162" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
+        <v>51</v>
+      </c>
+      <c r="B163" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C163" t="n">
+        <v>0</v>
+      </c>
+      <c r="D163" t="n">
+        <v>1</v>
+      </c>
+      <c r="E163" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>51</v>
+      </c>
+      <c r="B164" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C164" t="n">
+        <v>1</v>
+      </c>
+      <c r="D164" t="n">
+        <v>2</v>
+      </c>
+      <c r="E164" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>51</v>
+      </c>
+      <c r="B165" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C165" t="n">
+        <v>1</v>
+      </c>
+      <c r="D165" t="n">
+        <v>1</v>
+      </c>
+      <c r="E165" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>52</v>
+      </c>
+      <c r="B166" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C166" t="n">
+        <v>0</v>
+      </c>
+      <c r="D166" t="n">
+        <v>1</v>
+      </c>
+      <c r="E166" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>52</v>
+      </c>
+      <c r="B167" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C167" t="n">
+        <v>1</v>
+      </c>
+      <c r="D167" t="n">
+        <v>1</v>
+      </c>
+      <c r="E167" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s">
+        <v>7</v>
+      </c>
+      <c r="B168" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C168" t="n">
+        <v>2</v>
+      </c>
+      <c r="D168" t="n">
+        <v>3</v>
+      </c>
+      <c r="E168" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s">
+        <v>7</v>
+      </c>
+      <c r="B169" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C169" t="n">
+        <v>2</v>
+      </c>
+      <c r="D169" t="n">
+        <v>2</v>
+      </c>
+      <c r="E169" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>7</v>
+      </c>
+      <c r="B170" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C170" t="n">
+        <v>7</v>
+      </c>
+      <c r="D170" t="n">
+        <v>7</v>
+      </c>
+      <c r="E170" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>7</v>
+      </c>
+      <c r="B171" t="n">
+        <v>2024</v>
+      </c>
+      <c r="C171" t="n">
+        <v>1</v>
+      </c>
+      <c r="D171" t="n">
+        <v>1</v>
+      </c>
+      <c r="E171" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s">
+        <v>7</v>
+      </c>
+      <c r="B172" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C172" t="n">
+        <v>1</v>
+      </c>
+      <c r="D172" t="n">
+        <v>1</v>
+      </c>
+      <c r="E172" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s">
+        <v>53</v>
+      </c>
+      <c r="B173" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C173" t="n">
+        <v>3</v>
+      </c>
+      <c r="D173" t="n">
+        <v>3</v>
+      </c>
+      <c r="E173" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s">
+        <v>53</v>
+      </c>
+      <c r="B174" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C174" t="n">
+        <v>8</v>
+      </c>
+      <c r="D174" t="n">
+        <v>13</v>
+      </c>
+      <c r="E174" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s">
+        <v>53</v>
+      </c>
+      <c r="B175" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C175" t="n">
+        <v>8</v>
+      </c>
+      <c r="D175" t="n">
+        <v>8</v>
+      </c>
+      <c r="E175" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s">
+        <v>53</v>
+      </c>
+      <c r="B176" t="n">
+        <v>2024</v>
+      </c>
+      <c r="C176" t="n">
+        <v>13</v>
+      </c>
+      <c r="D176" t="n">
+        <v>15</v>
+      </c>
+      <c r="E176" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s">
+        <v>53</v>
+      </c>
+      <c r="B177" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C177" t="n">
+        <v>2</v>
+      </c>
+      <c r="D177" t="n">
+        <v>2</v>
+      </c>
+      <c r="E177" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s">
+        <v>54</v>
+      </c>
+      <c r="B178" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C178" t="n">
+        <v>1</v>
+      </c>
+      <c r="D178" t="n">
+        <v>1</v>
+      </c>
+      <c r="E178" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="s">
+        <v>54</v>
+      </c>
+      <c r="B179" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C179" t="n">
+        <v>3</v>
+      </c>
+      <c r="D179" t="n">
+        <v>3</v>
+      </c>
+      <c r="E179" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="s">
+        <v>54</v>
+      </c>
+      <c r="B180" t="n">
+        <v>2024</v>
+      </c>
+      <c r="C180" t="n">
+        <v>2</v>
+      </c>
+      <c r="D180" t="n">
+        <v>2</v>
+      </c>
+      <c r="E180" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="s">
         <v>55</v>
       </c>
-      <c r="B163" t="n">
+      <c r="B181" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C181" t="n">
+        <v>3</v>
+      </c>
+      <c r="D181" t="n">
+        <v>4</v>
+      </c>
+      <c r="E181" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="s">
+        <v>55</v>
+      </c>
+      <c r="B182" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C182" t="n">
+        <v>2</v>
+      </c>
+      <c r="D182" t="n">
+        <v>2</v>
+      </c>
+      <c r="E182" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s">
+        <v>55</v>
+      </c>
+      <c r="B183" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C183" t="n">
+        <v>4</v>
+      </c>
+      <c r="D183" t="n">
+        <v>5</v>
+      </c>
+      <c r="E183" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s">
+        <v>55</v>
+      </c>
+      <c r="B184" t="n">
         <v>2024</v>
       </c>
-      <c r="C163" t="n">
-        <v>2</v>
-      </c>
-      <c r="D163" t="n">
-        <v>2</v>
-      </c>
-      <c r="E163" t="n">
-        <v>2</v>
+      <c r="C184" t="n">
+        <v>2</v>
+      </c>
+      <c r="D184" t="n">
+        <v>2</v>
+      </c>
+      <c r="E184" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s">
+        <v>56</v>
+      </c>
+      <c r="B185" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C185" t="n">
+        <v>1</v>
+      </c>
+      <c r="D185" t="n">
+        <v>1</v>
+      </c>
+      <c r="E185" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>